<commit_message>
Actualizacion de tabla de precios en el documento
</commit_message>
<xml_diff>
--- a/Costos del proyecto.xlsx
+++ b/Costos del proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\FisgonParkingMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953B9590-9945-4C11-93EC-0FD472738CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F2A176-8794-4997-B792-450BF0A1353F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Equipos</t>
   </si>
@@ -97,6 +97,39 @@
   </si>
   <si>
     <t>Mano de obra</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Materiales y equipo</t>
+  </si>
+  <si>
+    <t>Especificaciones</t>
+  </si>
+  <si>
+    <t>Costos Adicionales</t>
+  </si>
+  <si>
+    <t>Calculo Final</t>
+  </si>
+  <si>
+    <t>Subtotal con baterías</t>
+  </si>
+  <si>
+    <t>Subtotal con fuente de poder</t>
+  </si>
+  <si>
+    <t>Beneficio módulos con batería</t>
+  </si>
+  <si>
+    <t>Beneficio módulos con fuente de poder</t>
+  </si>
+  <si>
+    <t>Costo total con batería</t>
+  </si>
+  <si>
+    <t>Costo total con fuente de poder</t>
   </si>
 </sst>
 </file>
@@ -106,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +167,13 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -176,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -274,6 +314,51 @@
         <color theme="0" tint="-0.499984740745262"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color theme="1"/>
       </top>
       <bottom style="thin">
@@ -282,6 +367,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -292,18 +392,18 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -311,23 +411,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,253 +760,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989EEDA1-F998-4775-A93A-FFC99F70D980}">
-  <dimension ref="C3:H25"/>
+  <dimension ref="C3:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.21875" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="3:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="7">
-        <v>5.76</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="D5" s="5">
+        <v>13.44</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <f>D5</f>
-        <v>5.76</v>
+        <v>13.44</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="G6" s="4" t="s">
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <f t="shared" ref="H6:H13" si="0">D6</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="G7" s="4" t="s">
+      <c r="D7" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="G8" s="4" t="s">
+      <c r="D8" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>12.3</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <f t="shared" si="0"/>
         <v>12.3</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="G10" s="4" t="s">
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="G11" s="4" t="s">
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>16</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="G13" s="4" t="s">
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>1.5</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>4.4649999999999999</v>
       </c>
     </row>
     <row r="15" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>3.3849999999999998</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="4">
         <f>SUM(H5:H14)</f>
-        <v>38.525000000000006</v>
+        <v>63.555000000000007</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <f>SUM(D5:D15)</f>
-        <v>38.945</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="3" t="s">
+        <v>63.975000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="16">
+        <v>32</v>
+      </c>
+      <c r="E23" s="4">
+        <f>D23*9</f>
+        <v>288</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <f>$E$23+E33+$E$24+$E$32</f>
+        <v>828.24</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="4">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="6">
+        <f>$E$23+E34+$E$24+$E$32</f>
+        <v>824.88000000000011</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="4">
+        <f>H23*D25</f>
+        <v>165.64800000000002</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="6">
+        <f>H23+E25</f>
+        <v>993.88800000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="4">
+        <f>H24*D26</f>
+        <v>164.97600000000003</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="6">
+        <f>H24+E26</f>
+        <v>989.85600000000011</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="18"/>
+    </row>
+    <row r="31" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E31" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
+    <row r="32" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D32" s="12">
         <v>1</v>
       </c>
-      <c r="E23" s="8">
-        <f>D5</f>
-        <v>5.76</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
+      <c r="E32" s="4">
+        <f>D5*D32</f>
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D33" s="13">
         <v>8</v>
       </c>
-      <c r="E24" s="8">
-        <f>D24*D16+E23</f>
-        <v>317.32</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
+      <c r="E33" s="4">
+        <f>D33*D16</f>
+        <v>511.8</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D34" s="14">
         <v>8</v>
       </c>
-      <c r="E25" s="8">
-        <f>D25*H15</f>
-        <v>308.20000000000005</v>
+      <c r="E34" s="4">
+        <f>D34*H15</f>
+        <v>508.44000000000005</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion de informacion en el documento en el apartado de pruebas y anexo
</commit_message>
<xml_diff>
--- a/Costos del proyecto.xlsx
+++ b/Costos del proyecto.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\FisgonParkingMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F2A176-8794-4997-B792-450BF0A1353F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DCEAE7-4822-429D-B0BA-9519A2001F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
+    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="1" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
+    <sheet name="Instalación" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Equipos</t>
   </si>
@@ -130,6 +131,39 @@
   </si>
   <si>
     <t>Costo total con fuente de poder</t>
+  </si>
+  <si>
+    <t>Tabla de instalación y funcionamiento</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Conexión física</t>
+  </si>
+  <si>
+    <t>Conexión local</t>
+  </si>
+  <si>
+    <t>Conexión Internet</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>✔</t>
+  </si>
+  <si>
+    <t>✘</t>
+  </si>
+  <si>
+    <t>El primer día de instalación se verificó el encendido con una red personal del autor pero no se logró conectar a la red del Instituto.</t>
+  </si>
+  <si>
+    <t>El segundo día se hicieron pruebas de conexión local sin éxito y la colocación del módulo prototipo en el puesto 3 del parqueadero.</t>
+  </si>
+  <si>
+    <t>Se instaló el módulo en el puesto 2 del parqueadero y fuente de energía para alimentación y se estableció conexión con la red del Instituto, la conexión suele ser debil y presenta algunos retrasos de la información en la página.</t>
   </si>
 </sst>
 </file>
@@ -139,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +211,16 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +257,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF124559"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF598392"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF495057"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -407,11 +473,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF202616"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF202616"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF202616"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF202616"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF202616"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF202616"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF202616"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF202616"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF202616"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF202616"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF202616"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -422,22 +531,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -446,12 +565,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCCC"/>
+      <color rgb="FF8E9AAF"/>
+      <color rgb="FF495057"/>
+      <color rgb="FFADB5BD"/>
+      <color rgb="FF979DAC"/>
+      <color rgb="FF7F9183"/>
+      <color rgb="FFBFC0C0"/>
+      <color rgb="FF598392"/>
+      <color rgb="FF124559"/>
+      <color rgb="FF202616"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -762,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989EEDA1-F998-4775-A93A-FFC99F70D980}">
   <dimension ref="C3:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView showGridLines="0" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,11 +913,15 @@
     <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="3:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
@@ -966,28 +1112,28 @@
     </row>
     <row r="20" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="17" t="s">
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="G21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="18"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="22" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="15" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -995,7 +1141,7 @@
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="15">
         <v>32</v>
       </c>
       <c r="E23" s="4">
@@ -1030,7 +1176,7 @@
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="10">
         <v>0.2</v>
       </c>
       <c r="E25" s="4">
@@ -1049,7 +1195,7 @@
       <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>0.2</v>
       </c>
       <c r="E26" s="4">
@@ -1066,20 +1212,20 @@
     </row>
     <row r="29" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="18"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
     </row>
     <row r="31" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1087,7 +1233,7 @@
       <c r="C32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <v>1</v>
       </c>
       <c r="E32" s="4">
@@ -1099,7 +1245,7 @@
       <c r="C33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="12">
         <v>8</v>
       </c>
       <c r="E33" s="4">
@@ -1111,7 +1257,7 @@
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="13">
         <v>8</v>
       </c>
       <c r="E34" s="4">
@@ -1130,4 +1276,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E035582-9F23-4A68-8A54-8D5A368E0998}">
+  <dimension ref="C5:G12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="27">
+        <v>45509</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="28">
+        <v>45510</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C11" s="28">
+        <v>45511</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C6:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Verificacion de la informacion
</commit_message>
<xml_diff>
--- a/Costos del proyecto.xlsx
+++ b/Costos del proyecto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\FisgonParkingMain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\FisgonParkingMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DCEAE7-4822-429D-B0BA-9519A2001F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733FB15-032F-4C22-959F-C3DD47795E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="1" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
+    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
@@ -21,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Equipos</t>
   </si>
@@ -164,6 +158,18 @@
   </si>
   <si>
     <t>Se instaló el módulo en el puesto 2 del parqueadero y fuente de energía para alimentación y se estableció conexión con la red del Instituto, la conexión suele ser debil y presenta algunos retrasos de la información en la página.</t>
+  </si>
+  <si>
+    <t>Selección de la PC adecuada.</t>
+  </si>
+  <si>
+    <t>Instalación de Windows en la PC.</t>
+  </si>
+  <si>
+    <t>Configuración de Windows para rendimiento.</t>
+  </si>
+  <si>
+    <t>Instalación y configuración del software de Ngrok.</t>
   </si>
 </sst>
 </file>
@@ -524,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -547,6 +553,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,12 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989EEDA1-F998-4775-A93A-FFC99F70D980}">
   <dimension ref="C3:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,8 +926,8 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="3:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
@@ -1112,21 +1118,21 @@
     </row>
     <row r="20" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23"/>
-      <c r="G21" s="21" t="s">
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="G21" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="23"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="14" t="s">
         <v>1</v>
       </c>
@@ -1212,11 +1218,11 @@
     </row>
     <row r="29" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C31" s="14" t="s">
@@ -1274,16 +1280,16 @@
     <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E035582-9F23-4A68-8A54-8D5A368E0998}">
-  <dimension ref="C5:G12"/>
+  <dimension ref="C5:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,20 +1302,20 @@
   <sheetData>
     <row r="5" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="16" t="s">
@@ -1329,7 +1335,7 @@
       </c>
     </row>
     <row r="9" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="27">
+      <c r="C9" s="20">
         <v>45509</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -1346,7 +1352,7 @@
       </c>
     </row>
     <row r="10" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C10" s="28">
+      <c r="C10" s="21">
         <v>45510</v>
       </c>
       <c r="D10" s="19" t="s">
@@ -1363,7 +1369,7 @@
       </c>
     </row>
     <row r="11" spans="3:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="28">
+      <c r="C11" s="21">
         <v>45511</v>
       </c>
       <c r="D11" s="19" t="s">
@@ -1380,17 +1386,91 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="28"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="17"/>
+      <c r="C12" s="21">
+        <v>45517</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="21">
+        <v>45518</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C14" s="21">
+        <v>45519</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="21">
+        <v>45520</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="21">
+        <v>45525</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion del manual y anexo del resultado de la instalacion
</commit_message>
<xml_diff>
--- a/Costos del proyecto.xlsx
+++ b/Costos del proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\FisgonParkingMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733FB15-032F-4C22-959F-C3DD47795E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41183C-D07B-479F-8FE6-B4FBE706486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Equipos</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Instalación y configuración del software de Ngrok.</t>
+  </si>
+  <si>
+    <t>Se instaló todo el sistema en la infraestructura y se probó su funcionamiento, con la observación que la infraestructura tiene carencias para la instalación completa del sistema.</t>
   </si>
 </sst>
 </file>
@@ -1288,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E035582-9F23-4A68-8A54-8D5A368E0998}">
   <dimension ref="C5:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1453,9 +1456,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C16" s="21">
-        <v>45525</v>
+        <v>45524</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>39</v>
@@ -1463,8 +1466,12 @@
       <c r="E16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="17"/>
+      <c r="F16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Presentacion añadida con cambios de costos y datos de manual
</commit_message>
<xml_diff>
--- a/Costos del proyecto.xlsx
+++ b/Costos del proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\FisgonParkingMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41183C-D07B-479F-8FE6-B4FBE706486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF46D3B-6A02-48B6-AEDF-158BD63BCA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
+    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989EEDA1-F998-4775-A93A-FFC99F70D980}">
   <dimension ref="C3:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="H23" s="6">
         <f>$E$23+E33+$E$24+$E$32</f>
-        <v>828.24</v>
+        <v>838.24</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1171,14 +1171,14 @@
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H24" s="6">
         <f>$E$23+E34+$E$24+$E$32</f>
-        <v>824.88000000000011</v>
+        <v>834.88000000000011</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1186,18 +1186,18 @@
         <v>29</v>
       </c>
       <c r="D25" s="10">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E25" s="4">
         <f>H23*D25</f>
-        <v>165.64800000000002</v>
+        <v>251.47199999999998</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H25" s="6">
         <f>H23+E25</f>
-        <v>993.88800000000003</v>
+        <v>1089.712</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1205,18 +1205,18 @@
         <v>30</v>
       </c>
       <c r="D26" s="10">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E26" s="4">
         <f>H24*D26</f>
-        <v>164.97600000000003</v>
+        <v>250.46400000000003</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H26" s="6">
         <f>H24+E26</f>
-        <v>989.85600000000011</v>
+        <v>1085.3440000000001</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1291,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E035582-9F23-4A68-8A54-8D5A368E0998}">
   <dimension ref="C5:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Actualizacion del repositorio 20/11/2024
</commit_message>
<xml_diff>
--- a/Costos del proyecto.xlsx
+++ b/Costos del proyecto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\FisgonParkingMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF46D3B-6A02-48B6-AEDF-158BD63BCA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2A0904-195F-41E5-B851-D21080C8B626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{97DB9E3C-2511-44AD-BF20-1115BDEF455C}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989EEDA1-F998-4775-A93A-FFC99F70D980}">
   <dimension ref="C3:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,15 +1189,15 @@
         <v>0.3</v>
       </c>
       <c r="E25" s="4">
-        <f>H23*D25</f>
-        <v>251.47199999999998</v>
+        <f>H23/(1-D25)-H23</f>
+        <v>359.24571428571426</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H25" s="6">
         <f>H23+E25</f>
-        <v>1089.712</v>
+        <v>1197.4857142857143</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1208,15 +1208,15 @@
         <v>0.3</v>
       </c>
       <c r="E26" s="4">
-        <f>H24*D26</f>
-        <v>250.46400000000003</v>
+        <f>H24/(1-D26)-H24</f>
+        <v>357.80571428571443</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H26" s="6">
         <f>H24+E26</f>
-        <v>1085.3440000000001</v>
+        <v>1192.6857142857145</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>

</xml_diff>